<commit_message>
Modify some test cases and adding class validations which contains all strings used in extent report test logs
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/TestData.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08AD7901-96ED-4847-80AB-680572553FE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF3340F-F9BE-4B3D-AB55-6B66BB5706B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9024" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
+    <workbookView xWindow="2790" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -646,21 +646,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CF6C07-F7D2-4879-98C8-38A47B6B27B6}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -668,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -676,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="12"/>
@@ -686,7 +686,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>13</v>
       </c>

</xml_diff>